<commit_message>
Análises de linha do tempo
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,10 +904,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -957,10 +955,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1010,10 +1006,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1063,10 +1057,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1113,6 +1105,218 @@
       </c>
       <c r="M13" t="n">
         <v>9.51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>12\09\24</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>qui</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>13:32:57</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Fortaleza</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>algumas nuvens</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>31.15</v>
+      </c>
+      <c r="H14" t="n">
+        <v>31.07</v>
+      </c>
+      <c r="I14" t="n">
+        <v>31.15</v>
+      </c>
+      <c r="J14" t="n">
+        <v>38.15</v>
+      </c>
+      <c r="K14" t="n">
+        <v>82</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1013</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>12\09\24</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>qui</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>13:32:57</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sobral</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>céu limpo</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>36.64</v>
+      </c>
+      <c r="H15" t="n">
+        <v>36.64</v>
+      </c>
+      <c r="I15" t="n">
+        <v>36.64</v>
+      </c>
+      <c r="J15" t="n">
+        <v>35.93</v>
+      </c>
+      <c r="K15" t="n">
+        <v>25</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1010</v>
+      </c>
+      <c r="M15" t="n">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>12\09\24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>qui</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>13:32:57</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Acaraú</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>céu limpo</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>29.81</v>
+      </c>
+      <c r="H16" t="n">
+        <v>29.81</v>
+      </c>
+      <c r="I16" t="n">
+        <v>29.81</v>
+      </c>
+      <c r="J16" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>58</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1011</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>12\09\24</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>qui</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>13:32:57</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Itarema</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>céu limpo</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="H17" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="I17" t="n">
+        <v>29.48</v>
+      </c>
+      <c r="J17" t="n">
+        <v>31.53</v>
+      </c>
+      <c r="K17" t="n">
+        <v>58</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1012</v>
+      </c>
+      <c r="M17" t="n">
+        <v>9.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>